<commit_message>
Completed formatting nad integration of Senior and Junior Report cards, Created Seperate page for Observable traits report. Formatted scores to reflect red:fail and Blue:pass. Tweeked Class setup to work with the working table (Changed  field names e.g class_id became classid, etc
</commit_message>
<xml_diff>
--- a/public/working/Scoresheet SSS/Further Mathematics.xlsx
+++ b/public/working/Scoresheet SSS/Further Mathematics.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scoresheet SSS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\schoolsmart\public\working\Scoresheet SSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CB6E377-7221-4096-9C15-90DC08869F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7F1E0D-02EC-4D7F-8E9D-8A005E72A556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECA4C89C-0668-41CD-8D73-BD07A005EDA0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ECA4C89C-0668-41CD-8D73-BD07A005EDA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
   <si>
     <t>ca1</t>
   </si>
@@ -201,6 +201,27 @@
   </si>
   <si>
     <t>FUTASEC00544</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>FMT</t>
+  </si>
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>session</t>
+  </si>
+  <si>
+    <t>created_at</t>
+  </si>
+  <si>
+    <t>updated_at</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -586,1687 +607,2103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FF215A-421D-4B75-8B03-8754B9F5BA88}">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A45"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="8.85546875" style="1"/>
-    <col min="6" max="6" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" style="1" customWidth="1"/>
+    <col min="4" max="7" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="O1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="1">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
+      <c r="E2" s="1">
         <v>19</v>
       </c>
-      <c r="D2" s="1">
+      <c r="F2" s="1">
         <v>19</v>
       </c>
-      <c r="E2" s="1">
-        <f t="shared" ref="E2:E45" si="0">SUM(25,D2)</f>
+      <c r="G2" s="1">
+        <f t="shared" ref="G2:G45" si="0">SUM(25,F2)</f>
         <v>44</v>
       </c>
-      <c r="F2" s="1">
-        <f t="shared" ref="F2:F45" si="1">SUM(B2,C2,D2,E2)</f>
+      <c r="H2" s="1">
+        <f t="shared" ref="H2:H45" si="1">SUM(D2,E2,F2,G2)</f>
         <v>90</v>
       </c>
-      <c r="G2" s="1">
-        <f t="shared" ref="G2:G45" si="2">SUM(-5,F2)</f>
+      <c r="I2" s="1">
+        <f t="shared" ref="I2:I45" si="2">SUM(-5,H2)</f>
         <v>85</v>
       </c>
-      <c r="H2" s="1">
-        <f t="shared" ref="H2:H45" si="3">AVERAGE(F2,G2)</f>
+      <c r="J2" s="1">
+        <f t="shared" ref="J2:J45" si="3">AVERAGE(H2,I2)</f>
         <v>87.5</v>
       </c>
-      <c r="I2" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="O2" s="1">
+        <v>2</v>
+      </c>
+      <c r="P2" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="1">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
+      <c r="E3" s="1">
         <v>17</v>
       </c>
-      <c r="D3" s="1">
-        <f>SUM(2,C3)</f>
+      <c r="F3" s="1">
+        <f>SUM(2,E3)</f>
         <v>19</v>
       </c>
-      <c r="E3" s="1">
+      <c r="G3" s="1">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="F3" s="1">
+      <c r="H3" s="1">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-      <c r="G3" s="1">
+      <c r="I3" s="1">
         <f t="shared" si="2"/>
         <v>83</v>
       </c>
-      <c r="H3" s="1">
+      <c r="J3" s="1">
         <f t="shared" si="3"/>
         <v>85.5</v>
       </c>
-      <c r="I3" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="K3" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L3" s="1">
+        <v>2</v>
+      </c>
+      <c r="O3" s="1">
+        <v>2</v>
+      </c>
+      <c r="P3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="1">
         <v>9</v>
       </c>
-      <c r="C4" s="1">
+      <c r="E4" s="1">
         <v>20</v>
       </c>
-      <c r="D4" s="1">
+      <c r="F4" s="1">
         <v>17</v>
       </c>
-      <c r="E4" s="1">
+      <c r="G4" s="1">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="F4" s="1">
+      <c r="H4" s="1">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-      <c r="G4" s="1">
+      <c r="I4" s="1">
         <f t="shared" si="2"/>
         <v>83</v>
       </c>
-      <c r="H4" s="1">
+      <c r="J4" s="1">
         <f t="shared" si="3"/>
         <v>85.5</v>
       </c>
-      <c r="I4" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J4" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="K4" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L4" s="1">
+        <v>3</v>
+      </c>
+      <c r="O4" s="1">
+        <v>2</v>
+      </c>
+      <c r="P4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="1">
         <v>8</v>
       </c>
-      <c r="C5" s="1">
+      <c r="E5" s="1">
         <v>20</v>
       </c>
-      <c r="D5" s="1">
+      <c r="F5" s="1">
         <v>17</v>
       </c>
-      <c r="E5" s="1">
+      <c r="G5" s="1">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="F5" s="1">
+      <c r="H5" s="1">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
-      <c r="G5" s="1">
+      <c r="I5" s="1">
         <f t="shared" si="2"/>
         <v>82</v>
       </c>
-      <c r="H5" s="1">
+      <c r="J5" s="1">
         <f t="shared" si="3"/>
         <v>84.5</v>
       </c>
-      <c r="I5" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="O5" s="1">
+        <v>2</v>
+      </c>
+      <c r="P5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="1">
         <v>6</v>
       </c>
-      <c r="C6" s="1">
+      <c r="E6" s="1">
         <v>17</v>
       </c>
-      <c r="D6" s="1">
-        <f>SUM(2,C6)</f>
+      <c r="F6" s="1">
+        <f>SUM(2,E6)</f>
         <v>19</v>
       </c>
-      <c r="E6" s="1">
+      <c r="G6" s="1">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="F6" s="1">
+      <c r="H6" s="1">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="G6" s="1">
+      <c r="I6" s="1">
         <f t="shared" si="2"/>
         <v>81</v>
       </c>
-      <c r="H6" s="1">
+      <c r="J6" s="1">
         <f t="shared" si="3"/>
         <v>83.5</v>
       </c>
-      <c r="I6" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L6" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="O6" s="1">
+        <v>2</v>
+      </c>
+      <c r="P6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1">
+      <c r="C7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="1">
         <v>9</v>
       </c>
-      <c r="C7" s="1">
+      <c r="E7" s="1">
         <v>19</v>
       </c>
-      <c r="D7" s="1">
+      <c r="F7" s="1">
         <v>16</v>
       </c>
-      <c r="E7" s="1">
+      <c r="G7" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="F7" s="1">
+      <c r="H7" s="1">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="G7" s="1">
+      <c r="I7" s="1">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="H7" s="1">
+      <c r="J7" s="1">
         <f t="shared" si="3"/>
         <v>82.5</v>
       </c>
-      <c r="I7" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L7" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="O7" s="1">
+        <v>2</v>
+      </c>
+      <c r="P7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1">
+      <c r="C8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="1">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
+      <c r="E8" s="1">
         <v>16</v>
       </c>
-      <c r="D8" s="1">
-        <f>SUM(2,C8)</f>
+      <c r="F8" s="1">
+        <f>SUM(2,E8)</f>
         <v>18</v>
       </c>
-      <c r="E8" s="1">
+      <c r="G8" s="1">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="F8" s="1">
+      <c r="H8" s="1">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="G8" s="1">
+      <c r="I8" s="1">
         <f t="shared" si="2"/>
         <v>79</v>
       </c>
-      <c r="H8" s="1">
+      <c r="J8" s="1">
         <f t="shared" si="3"/>
         <v>81.5</v>
       </c>
-      <c r="I8" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L8" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="O8" s="1">
+        <v>2</v>
+      </c>
+      <c r="P8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="1">
         <v>6</v>
       </c>
-      <c r="C9" s="1">
+      <c r="E9" s="1">
         <v>16</v>
       </c>
-      <c r="D9" s="1">
-        <f>SUM(2,C9)</f>
+      <c r="F9" s="1">
+        <f>SUM(2,E9)</f>
         <v>18</v>
       </c>
-      <c r="E9" s="1">
+      <c r="G9" s="1">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="F9" s="1">
+      <c r="H9" s="1">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-      <c r="G9" s="1">
+      <c r="I9" s="1">
         <f t="shared" si="2"/>
         <v>78</v>
       </c>
-      <c r="H9" s="1">
+      <c r="J9" s="1">
         <f t="shared" si="3"/>
         <v>80.5</v>
       </c>
-      <c r="I9" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L9" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="O9" s="1">
+        <v>2</v>
+      </c>
+      <c r="P9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="1">
         <v>8</v>
       </c>
-      <c r="C10" s="1">
+      <c r="E10" s="1">
         <v>15</v>
       </c>
-      <c r="D10" s="1">
-        <f>SUM(2,C10)</f>
+      <c r="F10" s="1">
+        <f>SUM(2,E10)</f>
         <v>17</v>
       </c>
-      <c r="E10" s="1">
+      <c r="G10" s="1">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="F10" s="1">
+      <c r="H10" s="1">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="G10" s="1">
+      <c r="I10" s="1">
         <f t="shared" si="2"/>
         <v>77</v>
       </c>
-      <c r="H10" s="1">
+      <c r="J10" s="1">
         <f t="shared" si="3"/>
         <v>79.5</v>
       </c>
-      <c r="I10" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L10" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="O10" s="1">
+        <v>2</v>
+      </c>
+      <c r="P10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1">
+      <c r="C11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="1">
         <v>5</v>
       </c>
-      <c r="C11" s="1">
+      <c r="E11" s="1">
         <v>16</v>
       </c>
-      <c r="D11" s="1">
-        <f>SUM(2,C11)</f>
+      <c r="F11" s="1">
+        <f>SUM(2,E11)</f>
         <v>18</v>
       </c>
-      <c r="E11" s="1">
+      <c r="G11" s="1">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="F11" s="1">
+      <c r="H11" s="1">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="G11" s="1">
+      <c r="I11" s="1">
         <f t="shared" si="2"/>
         <v>77</v>
       </c>
-      <c r="H11" s="1">
+      <c r="J11" s="1">
         <f t="shared" si="3"/>
         <v>79.5</v>
       </c>
-      <c r="I11" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L11" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="O11" s="1">
+        <v>2</v>
+      </c>
+      <c r="P11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1">
+      <c r="C12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="1">
         <v>4</v>
       </c>
-      <c r="C12" s="1">
+      <c r="E12" s="1">
         <v>16</v>
       </c>
-      <c r="D12" s="1">
-        <f>SUM(2,C12)</f>
+      <c r="F12" s="1">
+        <f>SUM(2,E12)</f>
         <v>18</v>
       </c>
-      <c r="E12" s="1">
+      <c r="G12" s="1">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="F12" s="1">
+      <c r="H12" s="1">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="G12" s="1">
+      <c r="I12" s="1">
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
-      <c r="H12" s="1">
+      <c r="J12" s="1">
         <f t="shared" si="3"/>
         <v>78.5</v>
       </c>
-      <c r="I12" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J12" s="1">
+      <c r="K12" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L12" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="O12" s="1">
+        <v>2</v>
+      </c>
+      <c r="P12" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1">
+      <c r="C13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="1">
         <v>6</v>
       </c>
-      <c r="C13" s="1">
+      <c r="E13" s="1">
         <v>15</v>
       </c>
-      <c r="D13" s="1">
+      <c r="F13" s="1">
         <v>17</v>
       </c>
-      <c r="E13" s="1">
+      <c r="G13" s="1">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="F13" s="1">
+      <c r="H13" s="1">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="G13" s="1">
+      <c r="I13" s="1">
         <f t="shared" si="2"/>
         <v>75</v>
       </c>
-      <c r="H13" s="1">
+      <c r="J13" s="1">
         <f t="shared" si="3"/>
         <v>77.5</v>
       </c>
-      <c r="I13" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J13" s="1">
+      <c r="K13" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L13" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="O13" s="1">
+        <v>2</v>
+      </c>
+      <c r="P13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="1">
+      <c r="C14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="1">
         <v>7</v>
       </c>
-      <c r="C14" s="1">
+      <c r="E14" s="1">
         <v>14</v>
       </c>
-      <c r="D14" s="1">
-        <f t="shared" ref="D14:D45" si="4">SUM(2,C14)</f>
+      <c r="F14" s="1">
+        <f t="shared" ref="F14:F45" si="4">SUM(2,E14)</f>
         <v>16</v>
       </c>
-      <c r="E14" s="1">
+      <c r="G14" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="F14" s="1">
+      <c r="H14" s="1">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-      <c r="G14" s="1">
+      <c r="I14" s="1">
         <f t="shared" si="2"/>
         <v>73</v>
       </c>
-      <c r="H14" s="1">
+      <c r="J14" s="1">
         <f t="shared" si="3"/>
         <v>75.5</v>
       </c>
-      <c r="I14" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J14" s="1">
+      <c r="K14" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L14" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="O14" s="1">
+        <v>2</v>
+      </c>
+      <c r="P14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="1">
+      <c r="C15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="1">
         <v>4</v>
       </c>
-      <c r="C15" s="1">
+      <c r="E15" s="1">
         <v>15</v>
       </c>
-      <c r="D15" s="1">
+      <c r="F15" s="1">
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="E15" s="1">
+      <c r="G15" s="1">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="F15" s="1">
+      <c r="H15" s="1">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-      <c r="G15" s="1">
+      <c r="I15" s="1">
         <f t="shared" si="2"/>
         <v>73</v>
       </c>
-      <c r="H15" s="1">
+      <c r="J15" s="1">
         <f t="shared" si="3"/>
         <v>75.5</v>
       </c>
-      <c r="I15" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J15" s="1">
+      <c r="K15" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L15" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="O15" s="1">
+        <v>2</v>
+      </c>
+      <c r="P15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="1">
+      <c r="C16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="1">
         <v>9</v>
       </c>
-      <c r="C16" s="1">
+      <c r="E16" s="1">
         <v>13</v>
       </c>
-      <c r="D16" s="1">
+      <c r="F16" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="E16" s="1">
+      <c r="G16" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="F16" s="1">
+      <c r="H16" s="1">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="G16" s="1">
+      <c r="I16" s="1">
         <f t="shared" si="2"/>
         <v>72</v>
       </c>
-      <c r="H16" s="1">
+      <c r="J16" s="1">
         <f t="shared" si="3"/>
         <v>74.5</v>
       </c>
-      <c r="I16" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J16" s="1">
+      <c r="K16" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L16" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="O16" s="1">
+        <v>2</v>
+      </c>
+      <c r="P16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="1">
-        <v>3</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="C17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1">
         <v>15</v>
       </c>
-      <c r="D17" s="1">
+      <c r="F17" s="1">
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="E17" s="1">
+      <c r="G17" s="1">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="F17" s="1">
+      <c r="H17" s="1">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="G17" s="1">
+      <c r="I17" s="1">
         <f t="shared" si="2"/>
         <v>72</v>
       </c>
-      <c r="H17" s="1">
+      <c r="J17" s="1">
         <f t="shared" si="3"/>
         <v>74.5</v>
       </c>
-      <c r="I17" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J17" s="1">
+      <c r="K17" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L17" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="O17" s="1">
+        <v>2</v>
+      </c>
+      <c r="P17" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="1">
+      <c r="C18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="1">
         <v>5</v>
       </c>
-      <c r="C18" s="1">
+      <c r="E18" s="1">
         <v>14</v>
       </c>
-      <c r="D18" s="1">
+      <c r="F18" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="E18" s="1">
+      <c r="G18" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="F18" s="1">
+      <c r="H18" s="1">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="G18" s="1">
+      <c r="I18" s="1">
         <f t="shared" si="2"/>
         <v>71</v>
       </c>
-      <c r="H18" s="1">
+      <c r="J18" s="1">
         <f t="shared" si="3"/>
         <v>73.5</v>
       </c>
-      <c r="I18" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J18" s="1">
+      <c r="K18" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L18" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="O18" s="1">
+        <v>2</v>
+      </c>
+      <c r="P18" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="1">
+      <c r="C19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="1">
         <v>4</v>
       </c>
-      <c r="C19" s="1">
+      <c r="E19" s="1">
         <v>14</v>
       </c>
-      <c r="D19" s="1">
+      <c r="F19" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="E19" s="1">
+      <c r="G19" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="F19" s="1">
+      <c r="H19" s="1">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="G19" s="1">
+      <c r="I19" s="1">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="H19" s="1">
+      <c r="J19" s="1">
         <f t="shared" si="3"/>
         <v>72.5</v>
       </c>
-      <c r="I19" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J19" s="1">
+      <c r="K19" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L19" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="O19" s="1">
+        <v>2</v>
+      </c>
+      <c r="P19" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="1">
+      <c r="C20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="1">
         <v>9</v>
       </c>
-      <c r="C20" s="1">
+      <c r="E20" s="1">
         <v>12</v>
       </c>
-      <c r="D20" s="1">
+      <c r="F20" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="E20" s="1">
+      <c r="G20" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="F20" s="1">
+      <c r="H20" s="1">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="G20" s="1">
+      <c r="I20" s="1">
         <f t="shared" si="2"/>
         <v>69</v>
       </c>
-      <c r="H20" s="1">
+      <c r="J20" s="1">
         <f t="shared" si="3"/>
         <v>71.5</v>
       </c>
-      <c r="I20" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J20" s="1">
+      <c r="K20" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L20" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="O20" s="1">
+        <v>2</v>
+      </c>
+      <c r="P20" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="1">
+      <c r="C21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="1">
         <v>9</v>
       </c>
-      <c r="C21" s="1">
+      <c r="E21" s="1">
         <v>12</v>
       </c>
-      <c r="D21" s="1">
+      <c r="F21" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="E21" s="1">
+      <c r="G21" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="F21" s="1">
+      <c r="H21" s="1">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="G21" s="1">
+      <c r="I21" s="1">
         <f t="shared" si="2"/>
         <v>69</v>
       </c>
-      <c r="H21" s="1">
+      <c r="J21" s="1">
         <f t="shared" si="3"/>
         <v>71.5</v>
       </c>
-      <c r="I21" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J21" s="1">
+      <c r="K21" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L21" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="O21" s="1">
+        <v>2</v>
+      </c>
+      <c r="P21" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="1">
-        <v>3</v>
-      </c>
-      <c r="C22" s="1">
+      <c r="C22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
+      <c r="E22" s="1">
         <v>14</v>
       </c>
-      <c r="D22" s="1">
+      <c r="F22" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="E22" s="1">
+      <c r="G22" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="F22" s="1">
+      <c r="H22" s="1">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="G22" s="1">
+      <c r="I22" s="1">
         <f t="shared" si="2"/>
         <v>69</v>
       </c>
-      <c r="H22" s="1">
+      <c r="J22" s="1">
         <f t="shared" si="3"/>
         <v>71.5</v>
       </c>
-      <c r="I22" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J22" s="1">
+      <c r="K22" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L22" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="O22" s="1">
+        <v>2</v>
+      </c>
+      <c r="P22" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="1">
+      <c r="C23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="1">
         <v>8</v>
       </c>
-      <c r="C23" s="1">
+      <c r="E23" s="1">
         <v>12</v>
       </c>
-      <c r="D23" s="1">
+      <c r="F23" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="E23" s="1">
+      <c r="G23" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="F23" s="1">
+      <c r="H23" s="1">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="G23" s="1">
+      <c r="I23" s="1">
         <f t="shared" si="2"/>
         <v>68</v>
       </c>
-      <c r="H23" s="1">
+      <c r="J23" s="1">
         <f t="shared" si="3"/>
         <v>70.5</v>
       </c>
-      <c r="I23" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J23" s="1">
+      <c r="K23" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L23" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="O23" s="1">
+        <v>2</v>
+      </c>
+      <c r="P23" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="1">
+      <c r="C24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="1">
         <v>5</v>
       </c>
-      <c r="C24" s="1">
+      <c r="E24" s="1">
         <v>13</v>
       </c>
-      <c r="D24" s="1">
+      <c r="F24" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="E24" s="1">
+      <c r="G24" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="F24" s="1">
+      <c r="H24" s="1">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="G24" s="1">
+      <c r="I24" s="1">
         <f t="shared" si="2"/>
         <v>68</v>
       </c>
-      <c r="H24" s="1">
+      <c r="J24" s="1">
         <f t="shared" si="3"/>
         <v>70.5</v>
       </c>
-      <c r="I24" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J24" s="1">
+      <c r="K24" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L24" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="O24" s="1">
+        <v>2</v>
+      </c>
+      <c r="P24" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="1">
+      <c r="C25" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="1">
         <v>4</v>
       </c>
-      <c r="C25" s="1">
+      <c r="E25" s="1">
         <v>13</v>
       </c>
-      <c r="D25" s="1">
+      <c r="F25" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="E25" s="1">
+      <c r="G25" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="F25" s="1">
+      <c r="H25" s="1">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="G25" s="1">
+      <c r="I25" s="1">
         <f t="shared" si="2"/>
         <v>67</v>
       </c>
-      <c r="H25" s="1">
+      <c r="J25" s="1">
         <f t="shared" si="3"/>
         <v>69.5</v>
       </c>
-      <c r="I25" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J25" s="1">
+      <c r="K25" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L25" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="O25" s="1">
+        <v>2</v>
+      </c>
+      <c r="P25" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="1">
+      <c r="C26" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="1">
         <v>7</v>
       </c>
-      <c r="C26" s="1">
+      <c r="E26" s="1">
         <v>12</v>
       </c>
-      <c r="D26" s="1">
+      <c r="F26" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="E26" s="1">
+      <c r="G26" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="F26" s="1">
+      <c r="H26" s="1">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="G26" s="1">
+      <c r="I26" s="1">
         <f t="shared" si="2"/>
         <v>67</v>
       </c>
-      <c r="H26" s="1">
+      <c r="J26" s="1">
         <f t="shared" si="3"/>
         <v>69.5</v>
       </c>
-      <c r="I26" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J26" s="1">
+      <c r="K26" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L26" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="O26" s="1">
+        <v>2</v>
+      </c>
+      <c r="P26" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B27" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="1">
+      <c r="C27" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="1">
         <v>6</v>
       </c>
-      <c r="C27" s="1">
+      <c r="E27" s="1">
         <v>12</v>
       </c>
-      <c r="D27" s="1">
+      <c r="F27" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="E27" s="1">
+      <c r="G27" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="F27" s="1">
+      <c r="H27" s="1">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="G27" s="1">
+      <c r="I27" s="1">
         <f t="shared" si="2"/>
         <v>66</v>
       </c>
-      <c r="H27" s="1">
+      <c r="J27" s="1">
         <f t="shared" si="3"/>
         <v>68.5</v>
       </c>
-      <c r="I27" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J27" s="1">
+      <c r="K27" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L27" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="O27" s="1">
+        <v>2</v>
+      </c>
+      <c r="P27" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="1">
-        <v>2</v>
-      </c>
-      <c r="C28" s="1">
+      <c r="C28" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1">
         <v>13</v>
       </c>
-      <c r="D28" s="1">
+      <c r="F28" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="E28" s="1">
+      <c r="G28" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="F28" s="1">
+      <c r="H28" s="1">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="G28" s="1">
+      <c r="I28" s="1">
         <f t="shared" si="2"/>
         <v>65</v>
       </c>
-      <c r="H28" s="1">
+      <c r="J28" s="1">
         <f t="shared" si="3"/>
         <v>67.5</v>
       </c>
-      <c r="I28" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J28" s="1">
+      <c r="K28" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L28" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="O28" s="1">
+        <v>2</v>
+      </c>
+      <c r="P28" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="1">
+      <c r="C29" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="1">
         <v>7</v>
       </c>
-      <c r="C29" s="1">
+      <c r="E29" s="1">
         <v>11</v>
       </c>
-      <c r="D29" s="1">
+      <c r="F29" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="E29" s="1">
+      <c r="G29" s="1">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="F29" s="1">
+      <c r="H29" s="1">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="G29" s="1">
+      <c r="I29" s="1">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="H29" s="1">
+      <c r="J29" s="1">
         <f t="shared" si="3"/>
         <v>66.5</v>
       </c>
-      <c r="I29" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J29" s="1">
+      <c r="K29" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L29" s="1">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="O29" s="1">
+        <v>2</v>
+      </c>
+      <c r="P29" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="1">
+      <c r="C30" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="1">
         <v>7</v>
       </c>
-      <c r="C30" s="1">
+      <c r="E30" s="1">
         <v>11</v>
       </c>
-      <c r="D30" s="1">
+      <c r="F30" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="E30" s="1">
+      <c r="G30" s="1">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="F30" s="1">
+      <c r="H30" s="1">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="G30" s="1">
+      <c r="I30" s="1">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="H30" s="1">
+      <c r="J30" s="1">
         <f t="shared" si="3"/>
         <v>66.5</v>
       </c>
-      <c r="I30" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J30" s="1">
+      <c r="K30" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L30" s="1">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="O30" s="1">
+        <v>2</v>
+      </c>
+      <c r="P30" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B31" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="1">
+      <c r="C31" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="1">
         <v>6</v>
       </c>
-      <c r="C31" s="1">
+      <c r="E31" s="1">
         <v>11</v>
       </c>
-      <c r="D31" s="1">
+      <c r="F31" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="E31" s="1">
+      <c r="G31" s="1">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="F31" s="1">
+      <c r="H31" s="1">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="G31" s="1">
+      <c r="I31" s="1">
         <f t="shared" si="2"/>
         <v>63</v>
       </c>
-      <c r="H31" s="1">
+      <c r="J31" s="1">
         <f t="shared" si="3"/>
         <v>65.5</v>
       </c>
-      <c r="I31" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J31" s="1">
+      <c r="K31" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L31" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="O31" s="1">
+        <v>2</v>
+      </c>
+      <c r="P31" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B32" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="1">
-        <v>3</v>
-      </c>
-      <c r="C32" s="1">
+      <c r="C32" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="1">
+        <v>3</v>
+      </c>
+      <c r="E32" s="1">
         <v>12</v>
       </c>
-      <c r="D32" s="1">
+      <c r="F32" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="E32" s="1">
+      <c r="G32" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="F32" s="1">
+      <c r="H32" s="1">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="G32" s="1">
+      <c r="I32" s="1">
         <f t="shared" si="2"/>
         <v>63</v>
       </c>
-      <c r="H32" s="1">
+      <c r="J32" s="1">
         <f t="shared" si="3"/>
         <v>65.5</v>
       </c>
-      <c r="I32" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J32" s="1">
+      <c r="K32" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L32" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="O32" s="1">
+        <v>2</v>
+      </c>
+      <c r="P32" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B33" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="1">
-        <v>3</v>
-      </c>
-      <c r="C33" s="1">
+      <c r="C33" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="1">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1">
         <v>12</v>
       </c>
-      <c r="D33" s="1">
+      <c r="F33" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="E33" s="1">
+      <c r="G33" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="F33" s="1">
+      <c r="H33" s="1">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="G33" s="1">
+      <c r="I33" s="1">
         <f t="shared" si="2"/>
         <v>63</v>
       </c>
-      <c r="H33" s="1">
+      <c r="J33" s="1">
         <f t="shared" si="3"/>
         <v>65.5</v>
       </c>
-      <c r="I33" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J33" s="1">
+      <c r="K33" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L33" s="1">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="O33" s="1">
+        <v>2</v>
+      </c>
+      <c r="P33" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B34" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="1">
+      <c r="C34" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="1">
         <v>8</v>
       </c>
-      <c r="C34" s="1">
+      <c r="E34" s="1">
         <v>10</v>
       </c>
-      <c r="D34" s="1">
+      <c r="F34" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="E34" s="1">
+      <c r="G34" s="1">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="F34" s="1">
+      <c r="H34" s="1">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
-      <c r="G34" s="1">
+      <c r="I34" s="1">
         <f t="shared" si="2"/>
         <v>62</v>
       </c>
-      <c r="H34" s="1">
+      <c r="J34" s="1">
         <f t="shared" si="3"/>
         <v>64.5</v>
       </c>
-      <c r="I34" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J34" s="1">
+      <c r="K34" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L34" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="O34" s="1">
+        <v>2</v>
+      </c>
+      <c r="P34" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B35" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="1">
+      <c r="C35" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="1">
         <v>4</v>
       </c>
-      <c r="C35" s="1">
+      <c r="E35" s="1">
         <v>11</v>
       </c>
-      <c r="D35" s="1">
+      <c r="F35" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="E35" s="1">
+      <c r="G35" s="1">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="F35" s="1">
+      <c r="H35" s="1">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
-      <c r="G35" s="1">
+      <c r="I35" s="1">
         <f t="shared" si="2"/>
         <v>61</v>
       </c>
-      <c r="H35" s="1">
+      <c r="J35" s="1">
         <f t="shared" si="3"/>
         <v>63.5</v>
       </c>
-      <c r="I35" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J35" s="1">
+      <c r="K35" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L35" s="1">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="O35" s="1">
+        <v>2</v>
+      </c>
+      <c r="P35" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B36" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="1">
+      <c r="C36" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="1">
         <v>9</v>
       </c>
-      <c r="C36" s="1">
+      <c r="E36" s="1">
         <v>9</v>
       </c>
-      <c r="D36" s="1">
+      <c r="F36" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="E36" s="1">
+      <c r="G36" s="1">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="F36" s="1">
+      <c r="H36" s="1">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="G36" s="1">
+      <c r="I36" s="1">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="H36" s="1">
+      <c r="J36" s="1">
         <f t="shared" si="3"/>
         <v>62.5</v>
       </c>
-      <c r="I36" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J36" s="1">
+      <c r="K36" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L36" s="1">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="O36" s="1">
+        <v>2</v>
+      </c>
+      <c r="P36" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B37" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="1">
+      <c r="C37" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="1">
         <v>5</v>
       </c>
-      <c r="C37" s="1">
+      <c r="E37" s="1">
         <v>10</v>
       </c>
-      <c r="D37" s="1">
+      <c r="F37" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="E37" s="1">
+      <c r="G37" s="1">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="F37" s="1">
+      <c r="H37" s="1">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="G37" s="1">
+      <c r="I37" s="1">
         <f t="shared" si="2"/>
         <v>59</v>
       </c>
-      <c r="H37" s="1">
+      <c r="J37" s="1">
         <f t="shared" si="3"/>
         <v>61.5</v>
       </c>
-      <c r="I37" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J37" s="1">
+      <c r="K37" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L37" s="1">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="O37" s="1">
+        <v>2</v>
+      </c>
+      <c r="P37" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B38" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="1">
-        <v>2</v>
-      </c>
-      <c r="C38" s="1">
+      <c r="C38" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="1">
+        <v>2</v>
+      </c>
+      <c r="E38" s="1">
         <v>11</v>
       </c>
-      <c r="D38" s="1">
+      <c r="F38" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="E38" s="1">
+      <c r="G38" s="1">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="F38" s="1">
+      <c r="H38" s="1">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="G38" s="1">
+      <c r="I38" s="1">
         <f t="shared" si="2"/>
         <v>59</v>
       </c>
-      <c r="H38" s="1">
+      <c r="J38" s="1">
         <f t="shared" si="3"/>
         <v>61.5</v>
       </c>
-      <c r="I38" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J38" s="1">
+      <c r="K38" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L38" s="1">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="O38" s="1">
+        <v>2</v>
+      </c>
+      <c r="P38" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B39" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B39" s="1">
+      <c r="C39" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" s="1">
         <v>5</v>
       </c>
-      <c r="C39" s="1">
+      <c r="E39" s="1">
         <v>10</v>
       </c>
-      <c r="D39" s="1">
+      <c r="F39" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="E39" s="1">
+      <c r="G39" s="1">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="F39" s="1">
+      <c r="H39" s="1">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="G39" s="1">
+      <c r="I39" s="1">
         <f t="shared" si="2"/>
         <v>59</v>
       </c>
-      <c r="H39" s="1">
+      <c r="J39" s="1">
         <f t="shared" si="3"/>
         <v>61.5</v>
       </c>
-      <c r="I39" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J39" s="1">
+      <c r="K39" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L39" s="1">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="O39" s="1">
+        <v>2</v>
+      </c>
+      <c r="P39" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B40" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="1">
-        <v>3</v>
-      </c>
-      <c r="C40" s="1">
+      <c r="C40" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="1">
+        <v>3</v>
+      </c>
+      <c r="E40" s="1">
         <v>10</v>
       </c>
-      <c r="D40" s="1">
+      <c r="F40" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="E40" s="1">
+      <c r="G40" s="1">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="F40" s="1">
+      <c r="H40" s="1">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="G40" s="1">
-        <f t="shared" si="2"/>
-        <v>57</v>
-      </c>
-      <c r="H40" s="1">
+      <c r="I40" s="1">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="J40" s="1">
         <f t="shared" si="3"/>
         <v>59.5</v>
       </c>
-      <c r="I40" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J40" s="1">
+      <c r="K40" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L40" s="1">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="O40" s="1">
+        <v>2</v>
+      </c>
+      <c r="P40" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B41" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="1">
+      <c r="C41" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" s="1">
         <v>6</v>
       </c>
-      <c r="C41" s="1">
+      <c r="E41" s="1">
         <v>9</v>
       </c>
-      <c r="D41" s="1">
+      <c r="F41" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="E41" s="1">
+      <c r="G41" s="1">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="F41" s="1">
+      <c r="H41" s="1">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="G41" s="1">
-        <f t="shared" si="2"/>
-        <v>57</v>
-      </c>
-      <c r="H41" s="1">
+      <c r="I41" s="1">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="J41" s="1">
         <f t="shared" si="3"/>
         <v>59.5</v>
       </c>
-      <c r="I41" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J41" s="1">
+      <c r="K41" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L41" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="O41" s="1">
+        <v>2</v>
+      </c>
+      <c r="P41" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B42" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B42" s="1">
+      <c r="C42" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" s="1">
         <v>4</v>
       </c>
-      <c r="C42" s="1">
+      <c r="E42" s="1">
         <v>9</v>
       </c>
-      <c r="D42" s="1">
+      <c r="F42" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="E42" s="1">
+      <c r="G42" s="1">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="F42" s="1">
+      <c r="H42" s="1">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="G42" s="1">
+      <c r="I42" s="1">
         <f t="shared" si="2"/>
         <v>55</v>
       </c>
-      <c r="H42" s="1">
+      <c r="J42" s="1">
         <f t="shared" si="3"/>
         <v>57.5</v>
       </c>
-      <c r="I42" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J42" s="1">
+      <c r="K42" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L42" s="1">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="O42" s="1">
+        <v>2</v>
+      </c>
+      <c r="P42" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B43" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B43" s="1">
+      <c r="C43" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43" s="1">
         <v>7</v>
       </c>
-      <c r="C43" s="1">
+      <c r="E43" s="1">
         <v>8</v>
       </c>
-      <c r="D43" s="1">
+      <c r="F43" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="E43" s="1">
+      <c r="G43" s="1">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="F43" s="1">
+      <c r="H43" s="1">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="G43" s="1">
+      <c r="I43" s="1">
         <f t="shared" si="2"/>
         <v>55</v>
       </c>
-      <c r="H43" s="1">
+      <c r="J43" s="1">
         <f t="shared" si="3"/>
         <v>57.5</v>
       </c>
-      <c r="I43" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J43" s="1">
+      <c r="K43" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L43" s="1">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="O43" s="1">
+        <v>2</v>
+      </c>
+      <c r="P43" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B44" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B44" s="1">
-        <v>3</v>
-      </c>
-      <c r="C44" s="1">
+      <c r="C44" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44" s="1">
+        <v>3</v>
+      </c>
+      <c r="E44" s="1">
         <v>9</v>
       </c>
-      <c r="D44" s="1">
+      <c r="F44" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="E44" s="1">
+      <c r="G44" s="1">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="F44" s="1">
+      <c r="H44" s="1">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="G44" s="1">
+      <c r="I44" s="1">
         <f t="shared" si="2"/>
         <v>54</v>
       </c>
-      <c r="H44" s="1">
+      <c r="J44" s="1">
         <f t="shared" si="3"/>
         <v>56.5</v>
       </c>
-      <c r="I44" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J44" s="1">
+      <c r="K44" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L44" s="1">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="O44" s="1">
+        <v>2</v>
+      </c>
+      <c r="P44" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B45" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B45" s="1">
+      <c r="C45" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45" s="1">
         <v>5</v>
       </c>
-      <c r="C45" s="1">
+      <c r="E45" s="1">
         <v>8</v>
       </c>
-      <c r="D45" s="1">
+      <c r="F45" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="E45" s="1">
+      <c r="G45" s="1">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="F45" s="1">
+      <c r="H45" s="1">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="G45" s="1">
+      <c r="I45" s="1">
         <f t="shared" si="2"/>
         <v>53</v>
       </c>
-      <c r="H45" s="1">
+      <c r="J45" s="1">
         <f t="shared" si="3"/>
         <v>55.5</v>
       </c>
-      <c r="I45" s="1">
-        <v>70.75</v>
-      </c>
-      <c r="J45" s="1">
+      <c r="K45" s="1">
+        <v>70.75</v>
+      </c>
+      <c r="L45" s="1">
         <v>44</v>
       </c>
+      <c r="O45" s="1">
+        <v>2</v>
+      </c>
+      <c r="P45" s="1">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L45">
-    <sortCondition descending="1" ref="H45"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:N45">
+    <sortCondition descending="1" ref="J45"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>